<commit_message>
[Carlos Retamales] - Anexando
</commit_message>
<xml_diff>
--- a/Encuesta.xlsx
+++ b/Encuesta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usachcl-my.sharepoint.com/personal/carlos_retamales_a_usach_cl/Documents/2022-2/8°Semestre/MINGESO/PEP_3/encuestados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usachcl-my.sharepoint.com/personal/carlos_retamales_a_usach_cl/Documents/2022-2/8°Semestre/MINGESO/PEP_3/Oficial/Mingeso_2022-2_PEP_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="580" documentId="8_{9ECBC618-0AE7-493F-BD79-D4726816A026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA52EBF1-AC5E-47FD-B381-8A7D0EFF0101}"/>
+  <xr:revisionPtr revIDLastSave="676" documentId="8_{9ECBC618-0AE7-493F-BD79-D4726816A026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FC0609D-C8D1-401D-B14E-708CECFB5269}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{5DD5CA30-D5EB-459D-9752-221271755DA0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5DD5CA30-D5EB-459D-9752-221271755DA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Perfiles" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="61">
   <si>
     <t>ID Participante</t>
   </si>
@@ -234,6 +234,15 @@
   </si>
   <si>
     <t>MALA</t>
+  </si>
+  <si>
+    <t>joe's pizza</t>
+  </si>
+  <si>
+    <t>localhost:5173</t>
+  </si>
+  <si>
+    <t>Joe's Pizza</t>
   </si>
 </sst>
 </file>
@@ -319,11 +328,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </top>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -360,25 +371,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -723,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A920543C-3461-4A4E-9BF5-0A18E4B0B5C0}">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -747,13 +756,13 @@
       <c r="D2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -958,10 +967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1860C81C-2862-424E-8837-807252FE0F11}">
-  <dimension ref="A2:P32"/>
+  <dimension ref="A2:P43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,13 +1020,13 @@
       <c r="M2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1115,7 +1124,7 @@
         <v>75</v>
       </c>
       <c r="N4" s="1" t="str">
-        <f t="shared" ref="N4:N32" si="0">IF(AND(M4&gt;=0,M4&lt;=62.6),"Detractor",IF(AND(M4&gt;62.6,M4&lt;=77.1),"Pasivo","Promotor"))</f>
+        <f t="shared" ref="N4:N37" si="0">IF(AND(M4&gt;=0,M4&lt;=62.6),"Detractor",IF(AND(M4&gt;62.6,M4&lt;=77.1),"Pasivo","Promotor"))</f>
         <v>Pasivo</v>
       </c>
       <c r="O4" s="5">
@@ -1163,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M6" si="1">(((C5+E5+G5+I5+K5)-5) + (25- (D5+F5+H5+J5+L5)))*2.5</f>
+        <f t="shared" ref="M5" si="1">(((C5+E5+G5+I5+K5)-5) + (25- (D5+F5+H5+J5+L5)))*2.5</f>
         <v>37.5</v>
       </c>
       <c r="N5" s="1" t="str">
@@ -1371,7 +1380,7 @@
         <v>2</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" ref="M7:M18" si="2">(((C9+E9+G9+I9+K9)-5) + (25- (D9+F9+H9+J9+L9)))*2.5</f>
+        <f t="shared" ref="M9:M16" si="2">(((C9+E9+G9+I9+K9)-5) + (25- (D9+F9+H9+J9+L9)))*2.5</f>
         <v>55</v>
       </c>
       <c r="N9" s="1" t="str">
@@ -1891,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" ref="M19:M32" si="3">(((C19+E19+G19+I19+K19)-5) + (25- (D19+F19+H19+J19+L19)))*2.5</f>
+        <f t="shared" ref="M19:M37" si="3">(((C19+E19+G19+I19+K19)-5) + (25- (D19+F19+H19+J19+L19)))*2.5</f>
         <v>75</v>
       </c>
       <c r="N19" s="1" t="str">
@@ -2002,7 +2011,7 @@
         <f t="shared" si="0"/>
         <v>Pasivo</v>
       </c>
-      <c r="O21" s="17">
+      <c r="O21" s="5">
         <v>7</v>
       </c>
       <c r="P21" s="5" t="s">
@@ -2054,7 +2063,7 @@
         <f t="shared" si="0"/>
         <v>Promotor</v>
       </c>
-      <c r="O22" s="17">
+      <c r="O22" s="5">
         <v>10</v>
       </c>
       <c r="P22" s="5" t="s">
@@ -2106,7 +2115,7 @@
         <f t="shared" si="0"/>
         <v>Promotor</v>
       </c>
-      <c r="O23" s="17">
+      <c r="O23" s="5">
         <v>6</v>
       </c>
       <c r="P23" s="5" t="s">
@@ -2365,6 +2374,359 @@
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
     </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
+        <v>1</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2</v>
+      </c>
+      <c r="H33" s="1">
+        <v>3</v>
+      </c>
+      <c r="I33" s="1">
+        <v>4</v>
+      </c>
+      <c r="J33" s="1">
+        <v>2</v>
+      </c>
+      <c r="K33" s="1">
+        <v>3</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="N33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Detractor</v>
+      </c>
+      <c r="O33" s="9">
+        <v>4</v>
+      </c>
+      <c r="P33" s="9"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="15">
+        <v>2</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1">
+        <v>3</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>3</v>
+      </c>
+      <c r="H34" s="1">
+        <v>3</v>
+      </c>
+      <c r="I34" s="1">
+        <v>3</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2</v>
+      </c>
+      <c r="K34" s="1">
+        <v>4</v>
+      </c>
+      <c r="L34" s="1">
+        <v>2</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="3"/>
+        <v>62.5</v>
+      </c>
+      <c r="N34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Detractor</v>
+      </c>
+      <c r="O34" s="9">
+        <v>3</v>
+      </c>
+      <c r="P34" s="9"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="15">
+        <v>3</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>4</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2</v>
+      </c>
+      <c r="I35" s="1">
+        <v>3</v>
+      </c>
+      <c r="J35" s="1">
+        <v>3</v>
+      </c>
+      <c r="K35" s="1">
+        <v>4</v>
+      </c>
+      <c r="L35" s="1">
+        <v>2</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="3"/>
+        <v>57.5</v>
+      </c>
+      <c r="N35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Detractor</v>
+      </c>
+      <c r="O35" s="9">
+        <v>4</v>
+      </c>
+      <c r="P35" s="9"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="15">
+        <v>4</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>5</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2</v>
+      </c>
+      <c r="H36" s="1">
+        <v>4</v>
+      </c>
+      <c r="I36" s="1">
+        <v>3</v>
+      </c>
+      <c r="J36" s="1">
+        <v>3</v>
+      </c>
+      <c r="K36" s="1">
+        <v>2</v>
+      </c>
+      <c r="L36" s="1">
+        <v>1</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="3"/>
+        <v>62.5</v>
+      </c>
+      <c r="N36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Detractor</v>
+      </c>
+      <c r="O36" s="9">
+        <v>3</v>
+      </c>
+      <c r="P36" s="9"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" s="15">
+        <v>5</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="1">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1">
+        <v>4</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2</v>
+      </c>
+      <c r="I37" s="1">
+        <v>4</v>
+      </c>
+      <c r="J37" s="1">
+        <v>1</v>
+      </c>
+      <c r="K37" s="1">
+        <v>3</v>
+      </c>
+      <c r="L37" s="5">
+        <v>1</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="3"/>
+        <v>67.5</v>
+      </c>
+      <c r="N37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Pasivo</v>
+      </c>
+      <c r="O37" s="9">
+        <v>6</v>
+      </c>
+      <c r="P37" s="9"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" s="15">
+        <v>6</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" s="15">
+        <v>7</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="15">
+        <v>8</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="15">
+        <v>9</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="15">
+        <v>10</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="14"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2375,8 +2737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF120417-CA28-4814-9A14-BFE0A23BFE1B}">
   <dimension ref="A2:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2406,16 +2768,16 @@
       <c r="E2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="7" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2449,7 +2811,7 @@
         <f>IF(AND(D3&gt;=0,D3&lt;=25),"[0-1,9]",IF(AND(D3&gt;25,D3&lt;=51.6),"[2-14]",IF(AND(D3&gt;51.6,D3&lt;=62.6),"[15-34]",IF(AND(D3&gt;62.6,D3&lt;=64.9),"[35-40]",IF(AND(D3&gt;64.9,D3&lt;=71),"[41-59]",IF(AND(D3&gt;71,D3&lt;=72.5),"[60-64]",IF(AND(D3&gt;72.5,D3&lt;=74),"[65-69]",IF(AND(D3&gt;74,D3&lt;=77.1),"[70-79]",IF(AND(D3&gt;77.1,D3&lt;=78.8),"[80-84]",IF(AND(D3&gt;78.8,D3&lt;=80.9),"[85-89]",IF(AND(D3&gt;80.9,D3&lt;=84),"[90-95]","[96-100]")))))))))))</f>
         <v>[41-59]</v>
       </c>
-      <c r="I3" s="15" cm="1">
+      <c r="I3" s="12" cm="1">
         <f t="array" ref="I3">AVERAGE(IF('Resultados encuesta'!B3:B23="pizzahut",'Resultados encuesta'!O3:O23))</f>
         <v>5.2857142857142856</v>
       </c>
@@ -2469,7 +2831,7 @@
         <v>82.5</v>
       </c>
       <c r="E4" s="5" t="str">
-        <f t="shared" ref="E4:E5" si="0">IF(D4&lt;50,"NO ACEPTABLE", IF(AND(D4&gt;=50,D4&lt;=70),"MARGINAL","ACEPTABLE"))</f>
+        <f t="shared" ref="E4:E6" si="0">IF(D4&lt;50,"NO ACEPTABLE", IF(AND(D4&gt;=50,D4&lt;=70),"MARGINAL","ACEPTABLE"))</f>
         <v>ACEPTABLE</v>
       </c>
       <c r="F4" s="5" t="str">
@@ -2481,10 +2843,10 @@
         <v>EXCELENTE</v>
       </c>
       <c r="H4" s="5" t="str">
-        <f t="shared" ref="H4:H5" si="2">IF(AND(D4&gt;=0,D4&lt;=25),"[0-1,9]",IF(AND(D4&gt;25,D4&lt;=51.6),"[2-14]",IF(AND(D4&gt;51.6,D4&lt;=62.6),"[15-34]",IF(AND(D4&gt;62.6,D4&lt;=64.9),"[35-40]",IF(AND(D4&gt;64.9,D4&lt;=71),"[41-59]",IF(AND(D4&gt;71,D4&lt;=72.5),"[60-64]",IF(AND(D4&gt;72.5,D4&lt;=74),"[65-69]",IF(AND(D4&gt;74,D4&lt;=77.1),"[70-79]",IF(AND(D4&gt;77.1,D4&lt;=78.8),"[80-84]",IF(AND(D4&gt;78.8,D4&lt;=80.9),"[85-89]",IF(AND(D4&gt;80.9,D4&lt;=84),"[90-95]","[96-100]")))))))))))</f>
+        <f t="shared" ref="H4:H6" si="2">IF(AND(D4&gt;=0,D4&lt;=25),"[0-1,9]",IF(AND(D4&gt;25,D4&lt;=51.6),"[2-14]",IF(AND(D4&gt;51.6,D4&lt;=62.6),"[15-34]",IF(AND(D4&gt;62.6,D4&lt;=64.9),"[35-40]",IF(AND(D4&gt;64.9,D4&lt;=71),"[41-59]",IF(AND(D4&gt;71,D4&lt;=72.5),"[60-64]",IF(AND(D4&gt;72.5,D4&lt;=74),"[65-69]",IF(AND(D4&gt;74,D4&lt;=77.1),"[70-79]",IF(AND(D4&gt;77.1,D4&lt;=78.8),"[80-84]",IF(AND(D4&gt;78.8,D4&lt;=80.9),"[85-89]",IF(AND(D4&gt;80.9,D4&lt;=84),"[90-95]","[96-100]")))))))))))</f>
         <v>[90-95]</v>
       </c>
-      <c r="I4" s="15" cm="1">
+      <c r="I4" s="12" cm="1">
         <f t="array" ref="I4">AVERAGE(IF('Resultados encuesta'!B3:B23="papajohns",'Resultados encuesta'!O3:O23))</f>
         <v>8.4285714285714288</v>
       </c>
@@ -2511,7 +2873,7 @@
         <f>IF(AND(D5&gt;=0,D5&lt;=51.6),"F",IF(AND(D5&gt;51.6,D5&lt;=62.6),"D",IF(AND(D5&gt;62.6,D5&lt;=64.9),"C-",IF(AND(D5&gt;64.9,D5&lt;=71),"C",IF(AND(D5&gt;71,D5&lt;=72.5),"C+",IF(AND(D5&gt;72.5,D5&lt;=74),"B-",IF(AND(D5&gt;74,D5&lt;=77.1),"B",IF(AND(D5&gt;77.1,D5&lt;=78.8),"B+",IF(AND(D5&gt;78.8,D5&lt;=80.9),"A-",IF(AND(D5&gt;80.9,D5&lt;=84),"A","A+"))))))))))</f>
         <v>C-</v>
       </c>
-      <c r="G5" s="13" t="str">
+      <c r="G5" s="11" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
@@ -2519,16 +2881,48 @@
         <f t="shared" si="2"/>
         <v>[35-40]</v>
       </c>
-      <c r="I5" s="15" cm="1">
+      <c r="I5" s="12" cm="1">
         <f t="array" ref="I5">AVERAGE(IF('Resultados encuesta'!B3:B23="dominospizza",'Resultados encuesta'!O3:O23))</f>
         <v>4.4285714285714288</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G6" s="14"/>
+      <c r="A6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="10" cm="1">
+        <f t="array" ref="D6">AVERAGE(IF('Resultados encuesta'!B33:B37="joe's pizza",'Resultados encuesta'!M33:M37))</f>
+        <v>62</v>
+      </c>
+      <c r="E6" s="5" t="str">
+        <f>IF(D6&lt;50,"NO ACEPTABLE", IF(AND(D6&gt;=50,D6&lt;=70),"MARGINAL","ACEPTABLE"))</f>
+        <v>MARGINAL</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <f>IF(AND(D6&gt;=0,D6&lt;=51.6),"F",IF(AND(D6&gt;51.6,D6&lt;=62.6),"D",IF(AND(D6&gt;62.6,D6&lt;=64.9),"C-",IF(AND(D6&gt;64.9,D6&lt;=71),"C",IF(AND(D6&gt;71,D6&lt;=72.5),"C+",IF(AND(D6&gt;72.5,D6&lt;=74),"B-",IF(AND(D6&gt;74,D6&lt;=77.1),"B",IF(AND(D6&gt;77.1,D6&lt;=78.8),"B+",IF(AND(D6&gt;78.8,D6&lt;=80.9),"A-",IF(AND(D6&gt;80.9,D6&lt;=84),"A","A+"))))))))))</f>
+        <v>D</v>
+      </c>
+      <c r="G6" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+      <c r="H6" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>[15-34]</v>
+      </c>
+      <c r="I6" s="12" cm="1">
+        <f t="array" ref="I6">AVERAGE(IF('Resultados encuesta'!B33:B37="joe's pizza",'Resultados encuesta'!O33:O37))</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="10">
@@ -2537,7 +2931,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3:E5">
+  <conditionalFormatting sqref="E3:E6">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO ACEPTABLE">
       <formula>NOT(ISERROR(SEARCH("NO ACEPTABLE",E3)))</formula>
     </cfRule>

</xml_diff>